<commit_message>
Datos Covid-19 Murcia 200614
</commit_message>
<xml_diff>
--- a/murcia/1. Datos a nivel regional.xlsx
+++ b/murcia/1. Datos a nivel regional.xlsx
@@ -283,8 +283,8 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4107,71 +4107,87 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H92" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
+      <c r="A92" s="1">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43995)</f>
+        <v>43995</v>
+      </c>
+      <c r="B92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69)</f>
+        <v>69</v>
+      </c>
+      <c r="C92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),59)</f>
+        <v>59</v>
+      </c>
+      <c r="D92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10)</f>
+        <v>10</v>
+      </c>
+      <c r="E92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3)</f>
+        <v>3</v>
+      </c>
+      <c r="F92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1413)</f>
+        <v>1413</v>
+      </c>
+      <c r="G92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),150)</f>
+        <v>150</v>
+      </c>
+      <c r="H92" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3190)</f>
+        <v>3190</v>
+      </c>
+      <c r="I92">
+        <f t="shared" ref="I92:I93" ca="1" si="18">+H92-H91</f>
+        <v>3</v>
+      </c>
+      <c r="J92">
+        <f t="shared" ref="J92:J93" ca="1" si="19">+F92-F91</f>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H93" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
+      <c r="A93" s="1">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43996)</f>
+        <v>43996</v>
+      </c>
+      <c r="B93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),68)</f>
+        <v>68</v>
+      </c>
+      <c r="C93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58)</f>
+        <v>58</v>
+      </c>
+      <c r="D93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10)</f>
+        <v>10</v>
+      </c>
+      <c r="E93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3)</f>
+        <v>3</v>
+      </c>
+      <c r="F93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1414)</f>
+        <v>1414</v>
+      </c>
+      <c r="G93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),150)</f>
+        <v>150</v>
+      </c>
+      <c r="H93" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3190)</f>
+        <v>3190</v>
+      </c>
+      <c r="I93">
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Excel Datos Covid-19 Murcia 200621
</commit_message>
<xml_diff>
--- a/murcia/1. Datos a nivel regional.xlsx
+++ b/murcia/1. Datos a nivel regional.xlsx
@@ -61,10 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,11 +281,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4191,242 +4192,253 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H94" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
+      <c r="A94" s="1">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43997)</f>
+        <v>43997</v>
+      </c>
+      <c r="B94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),68)</f>
+        <v>68</v>
+      </c>
+      <c r="C94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),60)</f>
+        <v>60</v>
+      </c>
+      <c r="D94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8)</f>
+        <v>8</v>
+      </c>
+      <c r="E94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2)</f>
+        <v>2</v>
+      </c>
+      <c r="F94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1414)</f>
+        <v>1414</v>
+      </c>
+      <c r="G94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),150)</f>
+        <v>150</v>
+      </c>
+      <c r="H94" s="2">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3190)</f>
+        <v>3190</v>
+      </c>
+      <c r="I94">
+        <f t="shared" ref="I94:I97" ca="1" si="20">+H94-H93</f>
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <f t="shared" ref="J94:J97" ca="1" si="21">+F94-F93</f>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H95" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
+      <c r="A95" s="1">
+        <v>43998</v>
+      </c>
+      <c r="B95" s="2">
+        <v>70</v>
+      </c>
+      <c r="C95" s="2">
+        <v>63</v>
+      </c>
+      <c r="D95" s="2">
+        <v>7</v>
+      </c>
+      <c r="E95" s="2">
+        <v>2</v>
+      </c>
+      <c r="F95" s="2">
+        <v>1414</v>
+      </c>
+      <c r="G95" s="2">
+        <v>150</v>
+      </c>
+      <c r="H95" s="2">
+        <v>3192</v>
+      </c>
+      <c r="I95">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J95">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H96" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H97" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H98" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H99" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="B100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="C100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="D100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="E100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="G100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="H100" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
+      <c r="A96" s="1">
+        <v>43999</v>
+      </c>
+      <c r="B96" s="2">
+        <v>74</v>
+      </c>
+      <c r="C96" s="2">
+        <v>67</v>
+      </c>
+      <c r="D96" s="2">
+        <v>7</v>
+      </c>
+      <c r="E96" s="2">
+        <v>2</v>
+      </c>
+      <c r="F96" s="2">
+        <v>1414</v>
+      </c>
+      <c r="G96" s="2">
+        <v>150</v>
+      </c>
+      <c r="H96" s="2">
+        <v>3202</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>44000</v>
+      </c>
+      <c r="B97" s="2">
+        <v>77</v>
+      </c>
+      <c r="C97" s="2">
+        <v>71</v>
+      </c>
+      <c r="D97" s="2">
+        <v>6</v>
+      </c>
+      <c r="E97" s="2">
+        <v>2</v>
+      </c>
+      <c r="F97" s="2">
+        <v>1414</v>
+      </c>
+      <c r="G97" s="2">
+        <v>150</v>
+      </c>
+      <c r="H97" s="2">
+        <v>3205</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>44001</v>
+      </c>
+      <c r="B98" s="2">
+        <v>83</v>
+      </c>
+      <c r="C98" s="2">
+        <v>76</v>
+      </c>
+      <c r="D98" s="2">
+        <v>7</v>
+      </c>
+      <c r="E98" s="2">
+        <v>2</v>
+      </c>
+      <c r="F98" s="2">
+        <v>1417</v>
+      </c>
+      <c r="G98" s="2">
+        <v>150</v>
+      </c>
+      <c r="H98" s="2">
+        <v>3211</v>
+      </c>
+      <c r="I98">
+        <f t="shared" ref="I98" si="22">+H98-H97</f>
+        <v>6</v>
+      </c>
+      <c r="J98">
+        <f t="shared" ref="J98" si="23">+F98-F97</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>44002</v>
+      </c>
+      <c r="B99" s="2">
+        <v>87</v>
+      </c>
+      <c r="C99" s="2">
+        <v>80</v>
+      </c>
+      <c r="D99" s="2">
+        <v>7</v>
+      </c>
+      <c r="E99" s="2">
+        <v>2</v>
+      </c>
+      <c r="F99" s="2">
+        <v>1418</v>
+      </c>
+      <c r="G99" s="2">
+        <v>150</v>
+      </c>
+      <c r="H99" s="2">
+        <v>3219</v>
+      </c>
+      <c r="I99">
+        <f t="shared" ref="I99" si="24">+H99-H98</f>
+        <v>8</v>
+      </c>
+      <c r="J99">
+        <f t="shared" ref="J99" si="25">+F99-F98</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>44003</v>
+      </c>
+      <c r="B100" s="2">
+        <v>69</v>
+      </c>
+      <c r="C100" s="2">
+        <v>62</v>
+      </c>
+      <c r="D100" s="2">
+        <v>7</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1440</v>
+      </c>
+      <c r="G100" s="2">
+        <v>150</v>
+      </c>
+      <c r="H100" s="2">
+        <v>3269</v>
+      </c>
+      <c r="I100">
+        <f t="shared" ref="I100" si="26">+H100-H99</f>
+        <v>50</v>
+      </c>
+      <c r="J100">
+        <f t="shared" ref="J100" si="27">+F100-F99</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F101" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>